<commit_message>
Update sourcing for bus bars
</commit_message>
<xml_diff>
--- a/procurement/bill-of-materials.xlsx
+++ b/procurement/bill-of-materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zbrozek-git\solarcar-batterypack\procurement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1772A30E-1595-4FBD-9A02-09FC5C8BEEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873C4282-B5BC-4CF7-A95E-5DC91763323E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="3850" windowWidth="23060" windowHeight="15160" xr2:uid="{D1D39CC7-F0DC-4302-817C-72372F10019E}"/>
+    <workbookView xWindow="4120" yWindow="4480" windowWidth="23060" windowHeight="15160" xr2:uid="{D1D39CC7-F0DC-4302-817C-72372F10019E}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
   <si>
     <t>Item</t>
   </si>
@@ -301,6 +301,33 @@
   </si>
   <si>
     <t>You can pick other values to suit your needs</t>
+  </si>
+  <si>
+    <t>Basic collector</t>
+  </si>
+  <si>
+    <t>End collector</t>
+  </si>
+  <si>
+    <t>End collector (mirrored)</t>
+  </si>
+  <si>
+    <t>Everbest Battery</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Order several spares, send .STEP to lily@everbestbattery.com</t>
+  </si>
+  <si>
+    <t>Order plenty of spares, send .STEP to lily@everbestbattery.com</t>
+  </si>
+  <si>
+    <t>Standard collector plate within cell stack</t>
+  </si>
+  <si>
+    <t>End terminal collector plate of cell stack</t>
   </si>
 </sst>
 </file>
@@ -358,21 +385,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -688,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35AEF16-A3B2-4455-A345-C04362318443}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -699,561 +727,621 @@
     <col min="1" max="1" width="12.08984375" customWidth="1"/>
     <col min="2" max="2" width="29.08984375" customWidth="1"/>
     <col min="3" max="3" width="44.81640625" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" customWidth="1"/>
     <col min="5" max="5" width="22.6328125" customWidth="1"/>
     <col min="6" max="6" width="41.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
-        <v>8</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
+        <v>30</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E7" s="5">
         <v>625515</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
         <v>2</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B14" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C14" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D14" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
         <v>1</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B15" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C15" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D15" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>1</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C16" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D16" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>1</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B17" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C17" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D17" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>4</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B18" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C18" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D18" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>4</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B19" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C19" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D19" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>1</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C20" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>64</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C21" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D21" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>64</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C22" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D22" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
         <v>32</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B23" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C23" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D23" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>32</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B24" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C24" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D24" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
         <v>128</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B25" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C25" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D25" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
         <v>8</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B26" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C26" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D26" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
         <v>1</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B27" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C27" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D27" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
         <v>1</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B28" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C28" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D28" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
         <v>32</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B29" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C29" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D29" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
         <v>1</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B30" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C30" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D30" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F30" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{5018EB06-6FF1-465A-8D5E-C20387C0F834}"/>
-    <hyperlink ref="E6" r:id="rId2" xr:uid="{AED5A16E-2FDD-4DFF-BFF5-DF187A08237E}"/>
-    <hyperlink ref="E7" r:id="rId3" xr:uid="{8CDFB7D7-2855-44EB-B3F8-1DC30B9FDF4F}"/>
-    <hyperlink ref="E8" r:id="rId4" xr:uid="{1341B924-4CE8-49B4-9879-70C36D703B9B}"/>
-    <hyperlink ref="E9" r:id="rId5" xr:uid="{DB715325-A5E8-4142-91C1-CB4D7671EAC4}"/>
-    <hyperlink ref="E10" r:id="rId6" xr:uid="{C9F8F54D-633F-4EC9-906D-512C3ECB3C9D}"/>
-    <hyperlink ref="E17" r:id="rId7" xr:uid="{5F669C13-254A-4366-88C8-AA954A1FD248}"/>
-    <hyperlink ref="E3" r:id="rId8" xr:uid="{1720EDB6-2970-4234-AE8D-A2EB8A1E4656}"/>
-    <hyperlink ref="E2" r:id="rId9" xr:uid="{7D9406DF-30E4-4CB4-BC64-6E5EF5394722}"/>
-    <hyperlink ref="E18" r:id="rId10" xr:uid="{A8CBEDD8-2E52-43E4-A6E4-AAC989359F3C}"/>
-    <hyperlink ref="E20" r:id="rId11" xr:uid="{00ED004B-BEF3-46D4-A9F1-5653CB0ECACE}"/>
-    <hyperlink ref="E21" r:id="rId12" xr:uid="{90BD5053-64C3-411A-824F-C52830C9ECEE}"/>
-    <hyperlink ref="E19" r:id="rId13" xr:uid="{08478DE1-4B7B-44A2-84F2-792CDB4E2BB7}"/>
-    <hyperlink ref="E13" r:id="rId14" xr:uid="{97BDC9BA-AA2A-4B79-9AF3-1FDB238A5DD8}"/>
-    <hyperlink ref="E11" r:id="rId15" xr:uid="{4D4ED1A0-014D-46E6-A815-F83D9669D738}"/>
-    <hyperlink ref="E15" r:id="rId16" xr:uid="{2A22CCB5-BC72-4BAA-BCEC-A4DC45084DBF}"/>
-    <hyperlink ref="E16" r:id="rId17" xr:uid="{762ABCE6-56DE-493E-8A2B-C9627A1FE13E}"/>
-    <hyperlink ref="E22" r:id="rId18" xr:uid="{AB1ACC5D-5ECA-4059-97DC-2E8EF8A5445D}"/>
-    <hyperlink ref="E12" r:id="rId19" xr:uid="{3222BA2C-3B4D-422B-8D97-181484BB8594}"/>
-    <hyperlink ref="E23" r:id="rId20" xr:uid="{053324CF-C718-4D69-AEFA-5147FC0FBCF2}"/>
-    <hyperlink ref="E24" r:id="rId21" xr:uid="{703C9D90-A3FF-4161-9E71-74EA7EEEA3AF}"/>
-    <hyperlink ref="E25" r:id="rId22" xr:uid="{79B816E4-8BA2-4BB2-B192-BE5E7BF8F531}"/>
-    <hyperlink ref="E4" r:id="rId23" display="https://www.homedepot.com/p/Frost-King-5-16-in-x-1-4-in-x-17-ft-Black-EPDM-Cellular-Rubber-Weatherstrip-Tape-V25BK/202844545" xr:uid="{FEA02C46-683D-40C3-8669-86F64F07737F}"/>
-    <hyperlink ref="E26" r:id="rId24" xr:uid="{0B4DDB7F-BCD6-433C-8493-C69541381BDE}"/>
-    <hyperlink ref="E14" r:id="rId25" xr:uid="{5D8DA4CF-D7DA-447D-A6E9-6C590F96EB07}"/>
-    <hyperlink ref="E27" r:id="rId26" xr:uid="{047ED4CC-5C21-4626-88F6-5FC8BF717D42}"/>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{5018EB06-6FF1-465A-8D5E-C20387C0F834}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{AED5A16E-2FDD-4DFF-BFF5-DF187A08237E}"/>
+    <hyperlink ref="E10" r:id="rId3" xr:uid="{8CDFB7D7-2855-44EB-B3F8-1DC30B9FDF4F}"/>
+    <hyperlink ref="E11" r:id="rId4" xr:uid="{1341B924-4CE8-49B4-9879-70C36D703B9B}"/>
+    <hyperlink ref="E12" r:id="rId5" xr:uid="{DB715325-A5E8-4142-91C1-CB4D7671EAC4}"/>
+    <hyperlink ref="E13" r:id="rId6" xr:uid="{C9F8F54D-633F-4EC9-906D-512C3ECB3C9D}"/>
+    <hyperlink ref="E20" r:id="rId7" xr:uid="{5F669C13-254A-4366-88C8-AA954A1FD248}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{1720EDB6-2970-4234-AE8D-A2EB8A1E4656}"/>
+    <hyperlink ref="E5" r:id="rId9" xr:uid="{7D9406DF-30E4-4CB4-BC64-6E5EF5394722}"/>
+    <hyperlink ref="E21" r:id="rId10" xr:uid="{A8CBEDD8-2E52-43E4-A6E4-AAC989359F3C}"/>
+    <hyperlink ref="E23" r:id="rId11" xr:uid="{00ED004B-BEF3-46D4-A9F1-5653CB0ECACE}"/>
+    <hyperlink ref="E24" r:id="rId12" xr:uid="{90BD5053-64C3-411A-824F-C52830C9ECEE}"/>
+    <hyperlink ref="E22" r:id="rId13" xr:uid="{08478DE1-4B7B-44A2-84F2-792CDB4E2BB7}"/>
+    <hyperlink ref="E16" r:id="rId14" xr:uid="{97BDC9BA-AA2A-4B79-9AF3-1FDB238A5DD8}"/>
+    <hyperlink ref="E14" r:id="rId15" xr:uid="{4D4ED1A0-014D-46E6-A815-F83D9669D738}"/>
+    <hyperlink ref="E18" r:id="rId16" xr:uid="{2A22CCB5-BC72-4BAA-BCEC-A4DC45084DBF}"/>
+    <hyperlink ref="E19" r:id="rId17" xr:uid="{762ABCE6-56DE-493E-8A2B-C9627A1FE13E}"/>
+    <hyperlink ref="E25" r:id="rId18" xr:uid="{AB1ACC5D-5ECA-4059-97DC-2E8EF8A5445D}"/>
+    <hyperlink ref="E15" r:id="rId19" xr:uid="{3222BA2C-3B4D-422B-8D97-181484BB8594}"/>
+    <hyperlink ref="E26" r:id="rId20" xr:uid="{053324CF-C718-4D69-AEFA-5147FC0FBCF2}"/>
+    <hyperlink ref="E27" r:id="rId21" xr:uid="{703C9D90-A3FF-4161-9E71-74EA7EEEA3AF}"/>
+    <hyperlink ref="E28" r:id="rId22" xr:uid="{79B816E4-8BA2-4BB2-B192-BE5E7BF8F531}"/>
+    <hyperlink ref="E7" r:id="rId23" display="https://www.homedepot.com/p/Frost-King-5-16-in-x-1-4-in-x-17-ft-Black-EPDM-Cellular-Rubber-Weatherstrip-Tape-V25BK/202844545" xr:uid="{FEA02C46-683D-40C3-8669-86F64F07737F}"/>
+    <hyperlink ref="E29" r:id="rId24" xr:uid="{0B4DDB7F-BCD6-433C-8493-C69541381BDE}"/>
+    <hyperlink ref="E17" r:id="rId25" xr:uid="{5D8DA4CF-D7DA-447D-A6E9-6C590F96EB07}"/>
+    <hyperlink ref="E30" r:id="rId26" xr:uid="{047ED4CC-5C21-4626-88F6-5FC8BF717D42}"/>
+    <hyperlink ref="D2" r:id="rId27" xr:uid="{5EA29408-AF76-4487-95D5-EBA6B359D47F}"/>
+    <hyperlink ref="D3" r:id="rId28" xr:uid="{96CB2BCC-A5EC-485B-9D31-0A951023FBEE}"/>
+    <hyperlink ref="D4" r:id="rId29" xr:uid="{8EEA5B90-7272-496A-8B8E-05147344EE67}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>